<commit_message>
-- exel import -- standatlaştırma
</commit_message>
<xml_diff>
--- a/backUp.xlsx
+++ b/backUp.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
   <si>
     <t>İSTANBUL 9.İCRA</t>
   </si>
@@ -196,6 +196,30 @@
   </si>
   <si>
     <t>BAKIRKÖY</t>
+  </si>
+  <si>
+    <t>ŞEHİR</t>
+  </si>
+  <si>
+    <t>İSTANBUL</t>
+  </si>
+  <si>
+    <t>ANKARA</t>
+  </si>
+  <si>
+    <t>ŞANLIURFA</t>
+  </si>
+  <si>
+    <t>DENİZLİ</t>
+  </si>
+  <si>
+    <t>İZMİR</t>
+  </si>
+  <si>
+    <t>BURSA</t>
+  </si>
+  <si>
+    <t>BALIKESİR</t>
   </si>
 </sst>
 </file>
@@ -588,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -602,12 +626,13 @@
     <col min="4" max="4" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="7" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -627,13 +652,16 @@
         <v>50</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,11 +681,14 @@
         <v>51</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -677,13 +708,16 @@
         <v>52</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -703,13 +737,16 @@
         <v>53</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -729,13 +766,16 @@
         <v>52</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -755,13 +795,16 @@
         <v>53</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -781,13 +824,16 @@
         <v>51</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -807,13 +853,16 @@
         <v>54</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -833,13 +882,16 @@
         <v>54</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -859,13 +911,16 @@
         <v>54</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -885,9 +940,12 @@
         <v>51</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>